<commit_message>
Pushing the new code
</commit_message>
<xml_diff>
--- a/DDT/Amazon user details.xlsx
+++ b/DDT/Amazon user details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satya\eclipse-workspace\Ecommerce_Amazon\DDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9EAF74-1ED0-4561-AB58-6EDA3B28D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD7BBE1-28FE-4AE4-8F95-CAC8052A004C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1960" windowWidth="14400" windowHeight="7270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserDetails1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Card Number</t>
+  </si>
+  <si>
+    <t>7676735387a</t>
   </si>
 </sst>
 </file>
@@ -430,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AFB30C-D722-4412-AF31-FB5122FD830E}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,8 +448,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>820009</v>
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -458,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB30D56E-4FF5-40F6-B9FE-81A96B2949BE}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>